<commit_message>
Author : Mannu Kumari Files Updated : GenerateReportController.java, GenerateReportDao.java, GenerateReportService.java, generateReport.yml, generateReportsCSS.css, generateReports.html, generateReportsContollerJS.js, Final Master Sheet.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/Documents/Excel Sheets/Final Master Sheet.xlsx
+++ b/Requirements/Documents/Excel Sheets/Final Master Sheet.xlsx
@@ -23,6 +23,7 @@
     <definedName name="Gender">'Drop Down values'!$H$2:$H$4</definedName>
     <definedName name="GuardianType">'Drop Down values'!$E$2:$E$5</definedName>
     <definedName name="ListOfStates">'Drop Down values'!$A$2:$A$33</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="PaymentMode">'Drop Down values'!$G$2</definedName>
     <definedName name="Salutation">'Drop Down values'!$D$2:$D$4</definedName>
   </definedNames>
@@ -2715,10 +2716,10 @@
     <t>PaymentMode</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>DD-MM-YYYY</t>
   </si>
 </sst>
 </file>
@@ -3524,9 +3525,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3676,7 +3677,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>25</v>
@@ -3755,7 +3756,7 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="11" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="8"/>

</xml_diff>